<commit_message>
terminamos con los requisitos nuevos y hacemos las issues
</commit_message>
<xml_diff>
--- a/guia/requisitos.xlsx
+++ b/guia/requisitos.xlsx
@@ -1,85 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="185">
-  <si>
-    <t xml:space="preserve">Código</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción corta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción larga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prioridad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complejidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entrega</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incidencia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estilo del código según las normas internas de Yii2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estilo del código según las normas internas de Yii2 para el código y para la plantilla de las vistas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mínimo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Técnico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fácil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">README.md</t>
-  </si>
-  <si>
-    <t xml:space="preserve">README.md en el directorio raíz con la descripción principal del proyecto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Documentación generada con yii2-apidoc</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="188">
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>Descripción corta</t>
+  </si>
+  <si>
+    <t>Descripción larga</t>
+  </si>
+  <si>
+    <t>Prioridad</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Complejidad</t>
+  </si>
+  <si>
+    <t>Entrega</t>
+  </si>
+  <si>
+    <t>Incidencia</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>Estilo del código según las normas internas de Yii2</t>
+  </si>
+  <si>
+    <t>Estilo del código según las normas internas de Yii2 para el código y para la plantilla de las vistas</t>
+  </si>
+  <si>
+    <t>Mínimo</t>
+  </si>
+  <si>
+    <t>Técnico</t>
+  </si>
+  <si>
+    <t>Fácil</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>README.md</t>
+  </si>
+  <si>
+    <t>README.md en el directorio raíz con la descripción principal del proyecto</t>
+  </si>
+  <si>
+    <t>R03</t>
+  </si>
+  <si>
+    <t>Documentación generada con yii2-apidoc</t>
   </si>
   <si>
     <t xml:space="preserve">Documentación generada con yii2-apidoc y publicada en GitHub Pages a partir del contenido del directorio /docs:
@@ -92,19 +87,19 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">R04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resolución de incidencias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Administración y resolución de todas las incidencias notificadas en GitHub.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La rama master reflejara el estado más estable</t>
+    <t>R04</t>
+  </si>
+  <si>
+    <t>resolución de incidencias</t>
+  </si>
+  <si>
+    <t>Administración y resolución de todas las incidencias notificadas en GitHub.</t>
+  </si>
+  <si>
+    <t>R05</t>
+  </si>
+  <si>
+    <t>La rama master reflejara el estado más estable</t>
   </si>
   <si>
     <t xml:space="preserve">La rama master debe reflejar en todo momento el estado más estable de la aplicación, de manera que:
@@ -115,223 +110,223 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">R06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usar Waffle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usar Waffle para la gestion general del proyecto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validación de  los campos de los formularios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de ventanas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de la apariencia de las ventanas. Creación de nuevas ventanas y comunicación entre ventanas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interactividad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interactividad  a través de mecanismos de manejo de eventos intuitivos y eficaces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uso y manipulación de las características del modelo de objetos del documento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mecanismos de almacenamiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uso de mecanismos de almacenamiento en el lado del cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JQUERY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uso de la librería JQUERY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plugins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incluir al menos un plugin no trabajado en clase.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AJAX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilización de mecanismos de comunicación asíncrona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHP 7.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yii2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yii2 Framework versión 2.0.10 ó superior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PostgreSQL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PostgreSQL versión 9.6 ó superior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heroku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Despliegue de la aplicación en la plataforma Heroku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Codeception</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pruebas funcionales con Codeception</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code climate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estilo y mantenibilidad del código fuente validados por Code Climate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aplicación escalable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La aplicación ha de ser escalable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTML5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Para estructurar el contenido se utilizarán las etiquetas semánticas de HTML5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSS3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Todo lo relacionado con la presentación se trabajará mediante CSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El diseño será flexible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contenido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Existirán transiciones, transformaciones, animaciones y contenido multimedia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uso de microdatos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resoluciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementar el diseño para resoluciones grandes y pequeñas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">navegadores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comprobar que el diseño es correcto en los siguientes navegadores:
+    <t>R06</t>
+  </si>
+  <si>
+    <t>Usar Waffle</t>
+  </si>
+  <si>
+    <t>Usar Waffle para la gestion general del proyecto</t>
+  </si>
+  <si>
+    <t>R07</t>
+  </si>
+  <si>
+    <t>Validación</t>
+  </si>
+  <si>
+    <t>Validación de  los campos de los formularios</t>
+  </si>
+  <si>
+    <t>R08</t>
+  </si>
+  <si>
+    <t>Gestión de ventanas</t>
+  </si>
+  <si>
+    <t>Gestión de la apariencia de las ventanas. Creación de nuevas ventanas y comunicación entre ventanas</t>
+  </si>
+  <si>
+    <t>R09</t>
+  </si>
+  <si>
+    <t>Interactividad</t>
+  </si>
+  <si>
+    <t>Interactividad  a través de mecanismos de manejo de eventos intuitivos y eficaces</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>DOM</t>
+  </si>
+  <si>
+    <t>Uso y manipulación de las características del modelo de objetos del documento</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>mecanismos de almacenamiento</t>
+  </si>
+  <si>
+    <t>Uso de mecanismos de almacenamiento en el lado del cliente</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>JQUERY</t>
+  </si>
+  <si>
+    <t>Uso de la librería JQUERY</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>plugins</t>
+  </si>
+  <si>
+    <t>Incluir al menos un plugin no trabajado en clase.</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>AJAX</t>
+  </si>
+  <si>
+    <t>Utilización de mecanismos de comunicación asíncrona</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>PHP 7.1</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>Yii2</t>
+  </si>
+  <si>
+    <t>Yii2 Framework versión 2.0.10 ó superior</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>PostgreSQL</t>
+  </si>
+  <si>
+    <t>PostgreSQL versión 9.6 ó superior</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>Heroku</t>
+  </si>
+  <si>
+    <t>Despliegue de la aplicación en la plataforma Heroku</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>Codeception</t>
+  </si>
+  <si>
+    <t>Pruebas funcionales con Codeception</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>Code climate</t>
+  </si>
+  <si>
+    <t>Estilo y mantenibilidad del código fuente validados por Code Climate</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>aplicación escalable</t>
+  </si>
+  <si>
+    <t>La aplicación ha de ser escalable</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>HTML5</t>
+  </si>
+  <si>
+    <t>Para estructurar el contenido se utilizarán las etiquetas semánticas de HTML5</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>CSS3</t>
+  </si>
+  <si>
+    <t>Todo lo relacionado con la presentación se trabajará mediante CSS</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>El diseño será flexible</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>Contenido</t>
+  </si>
+  <si>
+    <t>Existirán transiciones, transformaciones, animaciones y contenido multimedia</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>uso de microdatos</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>resoluciones</t>
+  </si>
+  <si>
+    <t>Implementar el diseño para resoluciones grandes y pequeñas.</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>navegadores</t>
+  </si>
+  <si>
+    <t>Comprobar que el diseño es correcto en los siguientes navegadores:
 Internet Explorer.
 Chrome.
 Mozilla Firefox.
 Opera.</t>
   </si>
   <si>
-    <t xml:space="preserve">R29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">despliegue en un Host</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realizar el despliegue en un Host:
+    <t>R29</t>
+  </si>
+  <si>
+    <t>despliegue en un Host</t>
+  </si>
+  <si>
+    <t>Realizar el despliegue en un Host:
 Utilizando algún servicio gratuito de hosting como los vistos en clase 
 Instalar / configurar o solicitar el software necesario para desplegar el proyecto.</t>
   </si>
   <si>
-    <t xml:space="preserve">R30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">despliegue en un servidor local</t>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>despliegue en un servidor local</t>
   </si>
   <si>
     <t xml:space="preserve">Realizar un despliegue en un servidor local usando y configurando tres máquinas virtuales para:
@@ -347,427 +342,1699 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">R31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usuarios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sobre los usuarios nos gustaría guardar el nombre de usuario, el correo, el teléfono móvil, el rol (según el rol que tenga podrá hacer unas cosas y otras no) y una referencia a la tabla alumno para el hijo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Importante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Información</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colegios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sobre los colegios nos interesa guardar el nombre del
+    <t>R31</t>
+  </si>
+  <si>
+    <t>Usuarios</t>
+  </si>
+  <si>
+    <t>Sobre los usuarios nos gustaría guardar el nombre de usuario, el correo, el teléfono móvil, el rol (según el rol que tenga podrá hacer unas cosas y otras no) y una referencia a la tabla alumno para el hijo</t>
+  </si>
+  <si>
+    <t>Importante</t>
+  </si>
+  <si>
+    <t>Información</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>Colegios</t>
+  </si>
+  <si>
+    <t>Sobre los colegios nos interesa guardar el nombre del
 Colegio, su cif y que usuario es su administrador</t>
   </si>
   <si>
-    <t xml:space="preserve">R33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alumnos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sobre los alumnos guardaríamos el nombre y los apellidos
+    <t>R33</t>
+  </si>
+  <si>
+    <t>Alumnos</t>
+  </si>
+  <si>
+    <t>Sobre los alumnos guardaríamos el nombre y los apellidos
 Del alumno, el curso y datos de contacto</t>
   </si>
   <si>
-    <t xml:space="preserve">R34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uniformes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guardaremos el tipo de uniforme, talla, el precio y colegio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stock seguridad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guardaremos datos para calcular stock de seguridad de
+    <t>R34</t>
+  </si>
+  <si>
+    <t>Uniformes</t>
+  </si>
+  <si>
+    <t>Guardaremos el tipo de uniforme, talla, el precio y colegio</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>Stock seguridad</t>
+  </si>
+  <si>
+    <t>Guardaremos datos para calcular stock de seguridad de
 Cada colegio</t>
   </si>
   <si>
-    <t xml:space="preserve">R36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Libros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guardaremos el ISBN, el titulo, el curso, el precio y colegio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facturas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guardaremos todos los datos de cada factura realizada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opcional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guardaremos registros de todos los mensajes SMS
+    <t>R36</t>
+  </si>
+  <si>
+    <t>Libros</t>
+  </si>
+  <si>
+    <t>Guardaremos el ISBN, el titulo, el curso, el precio y colegio</t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t>Facturas</t>
+  </si>
+  <si>
+    <t>Guardaremos todos los datos de cada factura realizada</t>
+  </si>
+  <si>
+    <t>Opcional</t>
+  </si>
+  <si>
+    <t>v3</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>Guardaremos registros de todos los mensajes SMS
 enviados con su fecha, numero destinatario y el mensaje</t>
   </si>
   <si>
-    <t xml:space="preserve">R39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Correos</t>
+    <t>R39</t>
+  </si>
+  <si>
+    <t>Correos</t>
   </si>
   <si>
     <t xml:space="preserve">Guardaremos registros de los mensajes de correo
 Enviados con la fecha, correo destinatario y el mensaje </t>
   </si>
   <si>
-    <t xml:space="preserve">R40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alta colegios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alta de los colegios por el administrador central</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Funcional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alta/baja usuarios aministradores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alta/baja de los administradores de cada colegio por el administrador central</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alta/baja usuarios vendedores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alta de los usuarios vendedores generados por los administradores de cada colegio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Importar datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Importar los datos de los uniformes, libros y alumno de un archivo externo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Media</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introducir datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduce los datos de los uniformes, libros y alumno mediante un formulario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestionar stock seguridad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introducir mediante formulario los datos para la gestión del stock de seguridad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consulta stock externo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consulta del stock de otros colegios por el usuario vendedor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hacer pedido externo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hacer pedido a otro colegio por el usuario vendedor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recibir pedido externo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Una vez realizado el pedido por parte de un usuario vendedor de un colegio el usuario vendedor del  colegio al que se le hace el pedido recibirá un aviso con los datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Darse de alta</t>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>Alta colegios</t>
+  </si>
+  <si>
+    <t>Alta de los colegios por el administrador central</t>
+  </si>
+  <si>
+    <t>Funcional</t>
+  </si>
+  <si>
+    <t>R41</t>
+  </si>
+  <si>
+    <t>Alta/baja usuarios aministradores</t>
+  </si>
+  <si>
+    <t>Alta/baja de los administradores de cada colegio por el administrador central</t>
+  </si>
+  <si>
+    <t>R42</t>
+  </si>
+  <si>
+    <t>Alta/baja usuarios vendedores</t>
+  </si>
+  <si>
+    <t>Alta de los usuarios vendedores generados por los administradores de cada colegio</t>
+  </si>
+  <si>
+    <t>R43</t>
+  </si>
+  <si>
+    <t>Importar datos</t>
+  </si>
+  <si>
+    <t>Importar los datos de los uniformes, libros y alumno de un archivo externo</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>R44</t>
+  </si>
+  <si>
+    <t>Introducir datos</t>
+  </si>
+  <si>
+    <t>Introduce los datos de los uniformes, libros y alumno mediante un formulario</t>
+  </si>
+  <si>
+    <t>R45</t>
+  </si>
+  <si>
+    <t>Gestionar stock seguridad</t>
+  </si>
+  <si>
+    <t>Introducir mediante formulario los datos para la gestión del stock de seguridad</t>
+  </si>
+  <si>
+    <t>R46</t>
+  </si>
+  <si>
+    <t>Consulta stock externo</t>
+  </si>
+  <si>
+    <t>Consulta del stock de otros colegios por el usuario vendedor</t>
+  </si>
+  <si>
+    <t>R47</t>
+  </si>
+  <si>
+    <t>Hacer pedido externo</t>
+  </si>
+  <si>
+    <t>Hacer pedido a otro colegio por el usuario vendedor</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>R48</t>
+  </si>
+  <si>
+    <t>Recibir pedido externo</t>
+  </si>
+  <si>
+    <t>Una vez realizado el pedido por parte de un usuario vendedor de un colegio el usuario vendedor del  colegio al que se le hace el pedido recibirá un aviso con los datos</t>
+  </si>
+  <si>
+    <t>R49</t>
+  </si>
+  <si>
+    <t>Darse de alta</t>
   </si>
   <si>
     <t xml:space="preserve">Alta de usuarios (padres) desde el portal a través de un formulario y comprobando que el hijo esta como alumno en dicho colegio </t>
   </si>
   <si>
-    <t xml:space="preserve">R50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hacer pedido interno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hacer pedido por el usuario padre a su colegio de libros o uniformes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recibir pedido interno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Una vez realizado el pedido por parte de un usuario padre el usuario vendedor de dicho colegio recibirá un aviso con los datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enviar SMS a administrador</t>
+    <t>R50</t>
+  </si>
+  <si>
+    <t>Hacer pedido interno</t>
+  </si>
+  <si>
+    <t>Hacer pedido por el usuario padre a su colegio de libros o uniformes</t>
+  </si>
+  <si>
+    <t>R51</t>
+  </si>
+  <si>
+    <t>Recibir pedido interno</t>
+  </si>
+  <si>
+    <t>Una vez realizado el pedido por parte de un usuario padre el usuario vendedor de dicho colegio recibirá un aviso con los datos</t>
+  </si>
+  <si>
+    <t>R52</t>
+  </si>
+  <si>
+    <t>Enviar SMS a administrador</t>
   </si>
   <si>
     <t xml:space="preserve">Envío de SMS a los administradores de cada colegio informándole de las alertas necesarias </t>
   </si>
   <si>
-    <t xml:space="preserve">Difícil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recordar contraseña</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En el caso de que el usuario padre se haya olvidado la contraseña, que al pulsar un botón se la mande por correo en el caso de haber hecho el requisito de enviar correos o por SMS en el caso contrario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enviar correo a vendedores</t>
+    <t>Difícil</t>
+  </si>
+  <si>
+    <t>R53</t>
+  </si>
+  <si>
+    <t>Recordar contraseña</t>
+  </si>
+  <si>
+    <t>En el caso de que el usuario padre se haya olvidado la contraseña, que al pulsar un botón se la mande por correo en el caso de haber hecho el requisito de enviar correos o por SMS en el caso contrario</t>
+  </si>
+  <si>
+    <t>R54</t>
+  </si>
+  <si>
+    <t>Enviar correo a vendedores</t>
   </si>
   <si>
     <t xml:space="preserve">Envío de correos a los vendedores de cada colegio informándole de las alertas necesarias </t>
   </si>
   <si>
-    <t xml:space="preserve">R55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facturación de uniformes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generación de factura con su correspondiente control en stock de los uniformes tanto a padres como a vendedores de otros colegios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alta/baja usuarios padre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alta de los usuarios padres generados por los usuarios administradores de colegio</t>
+    <t>R55</t>
+  </si>
+  <si>
+    <t>Facturación de uniformes</t>
+  </si>
+  <si>
+    <t>Generación de factura con su correspondiente control en stock de los uniformes tanto a padres como a vendedores de otros colegios</t>
+  </si>
+  <si>
+    <t>R56</t>
+  </si>
+  <si>
+    <t>Alta/baja usuarios padre</t>
+  </si>
+  <si>
+    <t>Alta de los usuarios padres generados por los usuarios administradores de colegio</t>
+  </si>
+  <si>
+    <t>R57</t>
+  </si>
+  <si>
+    <t>Tutores</t>
+  </si>
+  <si>
+    <t>Sobre los tutores guardaríamos sus datos personales como es el nombre, apellidos, dni, etc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="10">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:AMK59"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H57" activeCellId="0" sqref="H57"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="48.5969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="9.44897959183673"/>
+    <col min="1" max="1" width="9.3163265306122" customWidth="true" style="1"/>
+    <col min="2" max="2" width="18.224489795918" customWidth="true" style="2"/>
+    <col min="3" max="3" width="49.642857142857" customWidth="true" style="3"/>
+    <col min="4" max="4" width="9.3163265306122" customWidth="true" style="4"/>
+    <col min="5" max="5" width="10.663265306123" customWidth="true" style="4"/>
+    <col min="6" max="6" width="10.801020408163" customWidth="true" style="4"/>
+    <col min="7" max="7" width="9.3163265306122" customWidth="true" style="4"/>
+    <col min="8" max="8" width="9.3163265306122" customWidth="true" style="4"/>
+    <col min="9" max="9" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="10" max="10" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="11" max="11" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="12" max="12" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="13" max="13" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="14" max="14" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="15" max="15" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="16" max="16" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="17" max="17" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="18" max="18" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="19" max="19" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="20" max="20" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="21" max="21" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="22" max="22" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="23" max="23" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="24" max="24" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="25" max="25" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="26" max="26" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="27" max="27" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="28" max="28" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="29" max="29" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="30" max="30" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="31" max="31" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="32" max="32" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="33" max="33" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="34" max="34" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="35" max="35" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="36" max="36" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="37" max="37" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="38" max="38" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="39" max="39" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="40" max="40" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="41" max="41" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="42" max="42" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="43" max="43" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="44" max="44" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="45" max="45" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="46" max="46" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="47" max="47" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="48" max="48" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="49" max="49" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="50" max="50" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="51" max="51" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="52" max="52" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="53" max="53" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="54" max="54" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="55" max="55" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="56" max="56" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="57" max="57" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="58" max="58" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="59" max="59" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="60" max="60" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="61" max="61" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="62" max="62" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="63" max="63" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="64" max="64" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="65" max="65" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="66" max="66" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="67" max="67" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="68" max="68" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="69" max="69" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="70" max="70" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="71" max="71" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="72" max="72" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="73" max="73" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="74" max="74" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="75" max="75" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="76" max="76" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="77" max="77" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="78" max="78" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="79" max="79" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="80" max="80" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="81" max="81" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="82" max="82" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="83" max="83" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="84" max="84" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="85" max="85" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="86" max="86" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="87" max="87" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="88" max="88" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="89" max="89" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="90" max="90" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="91" max="91" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="92" max="92" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="93" max="93" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="94" max="94" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="95" max="95" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="96" max="96" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="97" max="97" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="98" max="98" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="99" max="99" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="100" max="100" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="101" max="101" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="102" max="102" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="103" max="103" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="104" max="104" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="105" max="105" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="106" max="106" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="107" max="107" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="108" max="108" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="109" max="109" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="110" max="110" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="111" max="111" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="112" max="112" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="113" max="113" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="114" max="114" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="115" max="115" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="116" max="116" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="117" max="117" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="118" max="118" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="119" max="119" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="120" max="120" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="121" max="121" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="122" max="122" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="123" max="123" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="124" max="124" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="125" max="125" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="126" max="126" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="127" max="127" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="128" max="128" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="129" max="129" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="130" max="130" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="131" max="131" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="132" max="132" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="133" max="133" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="134" max="134" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="135" max="135" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="136" max="136" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="137" max="137" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="138" max="138" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="139" max="139" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="140" max="140" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="141" max="141" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="142" max="142" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="143" max="143" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="144" max="144" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="145" max="145" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="146" max="146" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="147" max="147" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="148" max="148" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="149" max="149" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="150" max="150" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="151" max="151" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="152" max="152" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="153" max="153" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="154" max="154" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="155" max="155" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="156" max="156" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="157" max="157" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="158" max="158" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="159" max="159" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="160" max="160" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="161" max="161" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="162" max="162" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="163" max="163" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="164" max="164" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="165" max="165" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="166" max="166" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="167" max="167" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="168" max="168" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="169" max="169" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="170" max="170" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="171" max="171" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="172" max="172" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="173" max="173" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="174" max="174" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="175" max="175" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="176" max="176" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="177" max="177" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="178" max="178" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="179" max="179" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="180" max="180" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="181" max="181" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="182" max="182" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="183" max="183" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="184" max="184" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="185" max="185" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="186" max="186" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="187" max="187" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="188" max="188" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="189" max="189" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="190" max="190" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="191" max="191" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="192" max="192" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="193" max="193" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="194" max="194" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="195" max="195" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="196" max="196" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="197" max="197" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="198" max="198" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="199" max="199" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="200" max="200" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="201" max="201" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="202" max="202" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="203" max="203" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="204" max="204" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="205" max="205" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="206" max="206" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="207" max="207" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="208" max="208" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="209" max="209" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="210" max="210" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="211" max="211" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="212" max="212" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="213" max="213" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="214" max="214" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="215" max="215" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="216" max="216" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="217" max="217" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="218" max="218" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="219" max="219" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="220" max="220" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="221" max="221" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="222" max="222" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="223" max="223" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="224" max="224" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="225" max="225" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="226" max="226" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="227" max="227" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="228" max="228" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="229" max="229" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="230" max="230" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="231" max="231" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="232" max="232" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="233" max="233" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="234" max="234" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="235" max="235" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="236" max="236" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="237" max="237" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="238" max="238" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="239" max="239" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="240" max="240" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="241" max="241" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="242" max="242" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="243" max="243" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="244" max="244" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="245" max="245" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="246" max="246" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="247" max="247" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="248" max="248" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="249" max="249" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="250" max="250" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="251" max="251" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="252" max="252" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="253" max="253" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="254" max="254" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="255" max="255" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="256" max="256" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="257" max="257" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="258" max="258" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="259" max="259" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="260" max="260" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="261" max="261" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="262" max="262" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="263" max="263" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="264" max="264" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="265" max="265" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="266" max="266" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="267" max="267" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="268" max="268" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="269" max="269" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="270" max="270" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="271" max="271" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="272" max="272" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="273" max="273" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="274" max="274" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="275" max="275" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="276" max="276" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="277" max="277" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="278" max="278" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="279" max="279" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="280" max="280" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="281" max="281" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="282" max="282" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="283" max="283" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="284" max="284" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="285" max="285" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="286" max="286" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="287" max="287" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="288" max="288" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="289" max="289" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="290" max="290" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="291" max="291" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="292" max="292" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="293" max="293" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="294" max="294" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="295" max="295" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="296" max="296" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="297" max="297" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="298" max="298" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="299" max="299" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="300" max="300" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="301" max="301" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="302" max="302" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="303" max="303" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="304" max="304" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="305" max="305" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="306" max="306" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="307" max="307" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="308" max="308" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="309" max="309" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="310" max="310" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="311" max="311" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="312" max="312" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="313" max="313" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="314" max="314" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="315" max="315" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="316" max="316" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="317" max="317" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="318" max="318" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="319" max="319" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="320" max="320" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="321" max="321" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="322" max="322" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="323" max="323" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="324" max="324" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="325" max="325" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="326" max="326" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="327" max="327" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="328" max="328" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="329" max="329" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="330" max="330" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="331" max="331" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="332" max="332" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="333" max="333" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="334" max="334" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="335" max="335" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="336" max="336" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="337" max="337" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="338" max="338" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="339" max="339" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="340" max="340" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="341" max="341" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="342" max="342" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="343" max="343" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="344" max="344" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="345" max="345" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="346" max="346" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="347" max="347" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="348" max="348" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="349" max="349" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="350" max="350" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="351" max="351" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="352" max="352" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="353" max="353" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="354" max="354" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="355" max="355" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="356" max="356" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="357" max="357" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="358" max="358" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="359" max="359" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="360" max="360" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="361" max="361" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="362" max="362" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="363" max="363" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="364" max="364" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="365" max="365" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="366" max="366" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="367" max="367" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="368" max="368" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="369" max="369" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="370" max="370" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="371" max="371" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="372" max="372" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="373" max="373" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="374" max="374" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="375" max="375" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="376" max="376" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="377" max="377" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="378" max="378" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="379" max="379" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="380" max="380" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="381" max="381" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="382" max="382" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="383" max="383" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="384" max="384" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="385" max="385" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="386" max="386" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="387" max="387" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="388" max="388" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="389" max="389" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="390" max="390" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="391" max="391" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="392" max="392" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="393" max="393" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="394" max="394" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="395" max="395" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="396" max="396" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="397" max="397" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="398" max="398" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="399" max="399" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="400" max="400" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="401" max="401" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="402" max="402" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="403" max="403" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="404" max="404" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="405" max="405" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="406" max="406" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="407" max="407" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="408" max="408" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="409" max="409" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="410" max="410" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="411" max="411" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="412" max="412" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="413" max="413" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="414" max="414" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="415" max="415" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="416" max="416" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="417" max="417" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="418" max="418" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="419" max="419" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="420" max="420" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="421" max="421" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="422" max="422" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="423" max="423" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="424" max="424" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="425" max="425" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="426" max="426" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="427" max="427" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="428" max="428" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="429" max="429" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="430" max="430" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="431" max="431" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="432" max="432" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="433" max="433" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="434" max="434" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="435" max="435" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="436" max="436" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="437" max="437" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="438" max="438" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="439" max="439" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="440" max="440" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="441" max="441" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="442" max="442" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="443" max="443" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="444" max="444" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="445" max="445" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="446" max="446" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="447" max="447" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="448" max="448" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="449" max="449" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="450" max="450" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="451" max="451" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="452" max="452" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="453" max="453" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="454" max="454" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="455" max="455" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="456" max="456" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="457" max="457" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="458" max="458" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="459" max="459" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="460" max="460" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="461" max="461" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="462" max="462" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="463" max="463" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="464" max="464" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="465" max="465" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="466" max="466" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="467" max="467" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="468" max="468" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="469" max="469" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="470" max="470" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="471" max="471" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="472" max="472" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="473" max="473" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="474" max="474" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="475" max="475" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="476" max="476" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="477" max="477" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="478" max="478" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="479" max="479" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="480" max="480" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="481" max="481" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="482" max="482" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="483" max="483" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="484" max="484" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="485" max="485" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="486" max="486" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="487" max="487" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="488" max="488" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="489" max="489" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="490" max="490" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="491" max="491" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="492" max="492" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="493" max="493" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="494" max="494" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="495" max="495" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="496" max="496" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="497" max="497" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="498" max="498" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="499" max="499" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="500" max="500" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="501" max="501" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="502" max="502" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="503" max="503" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="504" max="504" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="505" max="505" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="506" max="506" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="507" max="507" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="508" max="508" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="509" max="509" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="510" max="510" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="511" max="511" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="512" max="512" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="513" max="513" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="514" max="514" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="515" max="515" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="516" max="516" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="517" max="517" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="518" max="518" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="519" max="519" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="520" max="520" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="521" max="521" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="522" max="522" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="523" max="523" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="524" max="524" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="525" max="525" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="526" max="526" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="527" max="527" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="528" max="528" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="529" max="529" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="530" max="530" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="531" max="531" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="532" max="532" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="533" max="533" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="534" max="534" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="535" max="535" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="536" max="536" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="537" max="537" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="538" max="538" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="539" max="539" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="540" max="540" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="541" max="541" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="542" max="542" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="543" max="543" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="544" max="544" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="545" max="545" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="546" max="546" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="547" max="547" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="548" max="548" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="549" max="549" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="550" max="550" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="551" max="551" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="552" max="552" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="553" max="553" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="554" max="554" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="555" max="555" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="556" max="556" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="557" max="557" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="558" max="558" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="559" max="559" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="560" max="560" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="561" max="561" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="562" max="562" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="563" max="563" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="564" max="564" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="565" max="565" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="566" max="566" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="567" max="567" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="568" max="568" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="569" max="569" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="570" max="570" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="571" max="571" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="572" max="572" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="573" max="573" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="574" max="574" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="575" max="575" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="576" max="576" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="577" max="577" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="578" max="578" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="579" max="579" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="580" max="580" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="581" max="581" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="582" max="582" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="583" max="583" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="584" max="584" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="585" max="585" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="586" max="586" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="587" max="587" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="588" max="588" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="589" max="589" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="590" max="590" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="591" max="591" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="592" max="592" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="593" max="593" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="594" max="594" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="595" max="595" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="596" max="596" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="597" max="597" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="598" max="598" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="599" max="599" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="600" max="600" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="601" max="601" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="602" max="602" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="603" max="603" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="604" max="604" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="605" max="605" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="606" max="606" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="607" max="607" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="608" max="608" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="609" max="609" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="610" max="610" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="611" max="611" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="612" max="612" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="613" max="613" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="614" max="614" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="615" max="615" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="616" max="616" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="617" max="617" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="618" max="618" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="619" max="619" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="620" max="620" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="621" max="621" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="622" max="622" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="623" max="623" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="624" max="624" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="625" max="625" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="626" max="626" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="627" max="627" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="628" max="628" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="629" max="629" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="630" max="630" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="631" max="631" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="632" max="632" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="633" max="633" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="634" max="634" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="635" max="635" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="636" max="636" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="637" max="637" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="638" max="638" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="639" max="639" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="640" max="640" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="641" max="641" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="642" max="642" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="643" max="643" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="644" max="644" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="645" max="645" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="646" max="646" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="647" max="647" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="648" max="648" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="649" max="649" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="650" max="650" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="651" max="651" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="652" max="652" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="653" max="653" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="654" max="654" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="655" max="655" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="656" max="656" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="657" max="657" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="658" max="658" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="659" max="659" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="660" max="660" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="661" max="661" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="662" max="662" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="663" max="663" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="664" max="664" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="665" max="665" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="666" max="666" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="667" max="667" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="668" max="668" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="669" max="669" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="670" max="670" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="671" max="671" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="672" max="672" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="673" max="673" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="674" max="674" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="675" max="675" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="676" max="676" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="677" max="677" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="678" max="678" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="679" max="679" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="680" max="680" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="681" max="681" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="682" max="682" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="683" max="683" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="684" max="684" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="685" max="685" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="686" max="686" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="687" max="687" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="688" max="688" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="689" max="689" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="690" max="690" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="691" max="691" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="692" max="692" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="693" max="693" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="694" max="694" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="695" max="695" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="696" max="696" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="697" max="697" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="698" max="698" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="699" max="699" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="700" max="700" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="701" max="701" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="702" max="702" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="703" max="703" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="704" max="704" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="705" max="705" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="706" max="706" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="707" max="707" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="708" max="708" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="709" max="709" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="710" max="710" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="711" max="711" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="712" max="712" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="713" max="713" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="714" max="714" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="715" max="715" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="716" max="716" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="717" max="717" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="718" max="718" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="719" max="719" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="720" max="720" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="721" max="721" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="722" max="722" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="723" max="723" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="724" max="724" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="725" max="725" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="726" max="726" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="727" max="727" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="728" max="728" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="729" max="729" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="730" max="730" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="731" max="731" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="732" max="732" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="733" max="733" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="734" max="734" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="735" max="735" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="736" max="736" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="737" max="737" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="738" max="738" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="739" max="739" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="740" max="740" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="741" max="741" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="742" max="742" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="743" max="743" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="744" max="744" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="745" max="745" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="746" max="746" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="747" max="747" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="748" max="748" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="749" max="749" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="750" max="750" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="751" max="751" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="752" max="752" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="753" max="753" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="754" max="754" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="755" max="755" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="756" max="756" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="757" max="757" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="758" max="758" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="759" max="759" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="760" max="760" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="761" max="761" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="762" max="762" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="763" max="763" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="764" max="764" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="765" max="765" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="766" max="766" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="767" max="767" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="768" max="768" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="769" max="769" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="770" max="770" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="771" max="771" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="772" max="772" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="773" max="773" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="774" max="774" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="775" max="775" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="776" max="776" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="777" max="777" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="778" max="778" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="779" max="779" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="780" max="780" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="781" max="781" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="782" max="782" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="783" max="783" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="784" max="784" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="785" max="785" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="786" max="786" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="787" max="787" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="788" max="788" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="789" max="789" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="790" max="790" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="791" max="791" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="792" max="792" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="793" max="793" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="794" max="794" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="795" max="795" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="796" max="796" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="797" max="797" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="798" max="798" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="799" max="799" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="800" max="800" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="801" max="801" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="802" max="802" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="803" max="803" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="804" max="804" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="805" max="805" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="806" max="806" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="807" max="807" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="808" max="808" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="809" max="809" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="810" max="810" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="811" max="811" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="812" max="812" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="813" max="813" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="814" max="814" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="815" max="815" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="816" max="816" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="817" max="817" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="818" max="818" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="819" max="819" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="820" max="820" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="821" max="821" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="822" max="822" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="823" max="823" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="824" max="824" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="825" max="825" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="826" max="826" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="827" max="827" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="828" max="828" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="829" max="829" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="830" max="830" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="831" max="831" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="832" max="832" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="833" max="833" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="834" max="834" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="835" max="835" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="836" max="836" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="837" max="837" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="838" max="838" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="839" max="839" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="840" max="840" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="841" max="841" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="842" max="842" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="843" max="843" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="844" max="844" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="845" max="845" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="846" max="846" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="847" max="847" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="848" max="848" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="849" max="849" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="850" max="850" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="851" max="851" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="852" max="852" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="853" max="853" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="854" max="854" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="855" max="855" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="856" max="856" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="857" max="857" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="858" max="858" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="859" max="859" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="860" max="860" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="861" max="861" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="862" max="862" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="863" max="863" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="864" max="864" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="865" max="865" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="866" max="866" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="867" max="867" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="868" max="868" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="869" max="869" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="870" max="870" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="871" max="871" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="872" max="872" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="873" max="873" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="874" max="874" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="875" max="875" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="876" max="876" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="877" max="877" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="878" max="878" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="879" max="879" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="880" max="880" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="881" max="881" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="882" max="882" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="883" max="883" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="884" max="884" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="885" max="885" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="886" max="886" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="887" max="887" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="888" max="888" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="889" max="889" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="890" max="890" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="891" max="891" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="892" max="892" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="893" max="893" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="894" max="894" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="895" max="895" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="896" max="896" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="897" max="897" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="898" max="898" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="899" max="899" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="900" max="900" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="901" max="901" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="902" max="902" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="903" max="903" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="904" max="904" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="905" max="905" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="906" max="906" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="907" max="907" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="908" max="908" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="909" max="909" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="910" max="910" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="911" max="911" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="912" max="912" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="913" max="913" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="914" max="914" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="915" max="915" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="916" max="916" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="917" max="917" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="918" max="918" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="919" max="919" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="920" max="920" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="921" max="921" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="922" max="922" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="923" max="923" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="924" max="924" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="925" max="925" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="926" max="926" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="927" max="927" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="928" max="928" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="929" max="929" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="930" max="930" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="931" max="931" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="932" max="932" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="933" max="933" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="934" max="934" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="935" max="935" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="936" max="936" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="937" max="937" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="938" max="938" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="939" max="939" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="940" max="940" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="941" max="941" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="942" max="942" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="943" max="943" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="944" max="944" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="945" max="945" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="946" max="946" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="947" max="947" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="948" max="948" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="949" max="949" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="950" max="950" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="951" max="951" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="952" max="952" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="953" max="953" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="954" max="954" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="955" max="955" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="956" max="956" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="957" max="957" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="958" max="958" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="959" max="959" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="960" max="960" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="961" max="961" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="962" max="962" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="963" max="963" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="964" max="964" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="965" max="965" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="966" max="966" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="967" max="967" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="968" max="968" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="969" max="969" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="970" max="970" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="971" max="971" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="972" max="972" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="973" max="973" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="974" max="974" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="975" max="975" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="976" max="976" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="977" max="977" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="978" max="978" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="979" max="979" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="980" max="980" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="981" max="981" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="982" max="982" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="983" max="983" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="984" max="984" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="985" max="985" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="986" max="986" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="987" max="987" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="988" max="988" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="989" max="989" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="990" max="990" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="991" max="991" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="992" max="992" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="993" max="993" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="994" max="994" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="995" max="995" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="996" max="996" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="997" max="997" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="998" max="998" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="999" max="999" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1000" max="1000" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1001" max="1001" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1002" max="1002" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1003" max="1003" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1004" max="1004" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1005" max="1005" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1006" max="1006" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1007" max="1007" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1008" max="1008" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1009" max="1009" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1010" max="1010" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1011" max="1011" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1012" max="1012" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1013" max="1013" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1014" max="1014" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1015" max="1015" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1016" max="1016" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1017" max="1017" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1018" max="1018" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1019" max="1019" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1020" max="1020" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1021" max="1021" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1022" max="1022" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1023" max="1023" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1024" max="1024" width="9.3163265306122" customWidth="true" style="5"/>
+    <col min="1025" max="1025" width="9.3163265306122" customWidth="true" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -793,7 +2060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="34.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:1025" customHeight="1" ht="34.95">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -815,11 +2082,11 @@
       <c r="G2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:1025" customHeight="1" ht="23.7">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -841,11 +2108,11 @@
       <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="158.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:1025" customHeight="1" ht="158.7">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -867,11 +2134,11 @@
       <c r="G4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:1025" customHeight="1" ht="23.7">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -893,11 +2160,11 @@
       <c r="G5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="181.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:1025" customHeight="1" ht="181.2">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -919,11 +2186,11 @@
       <c r="G6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -945,11 +2212,11 @@
       <c r="G7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -971,11 +2238,11 @@
       <c r="G8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:1025" customHeight="1" ht="23.7">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -997,11 +2264,11 @@
       <c r="G9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:1025" customHeight="1" ht="23.7">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1023,11 +2290,11 @@
       <c r="G10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:1025" customHeight="1" ht="23.7">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -1049,11 +2316,11 @@
       <c r="G11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:1025" customHeight="1" ht="23.7">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -1075,11 +2342,11 @@
       <c r="G12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -1101,11 +2368,11 @@
       <c r="G13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -1127,11 +2394,11 @@
       <c r="G14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
@@ -1153,11 +2420,11 @@
       <c r="G15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -1179,11 +2446,11 @@
       <c r="G16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -1205,11 +2472,11 @@
       <c r="G17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A18" s="1" t="s">
         <v>59</v>
       </c>
@@ -1231,11 +2498,11 @@
       <c r="G18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
@@ -1257,11 +2524,11 @@
       <c r="G19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
@@ -1283,11 +2550,11 @@
       <c r="G20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:1025" customHeight="1" ht="23.7">
       <c r="A21" s="1" t="s">
         <v>68</v>
       </c>
@@ -1309,11 +2576,11 @@
       <c r="G21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A22" s="1" t="s">
         <v>71</v>
       </c>
@@ -1335,11 +2602,11 @@
       <c r="G22" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:1025" customHeight="1" ht="23.7">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -1361,11 +2628,11 @@
       <c r="G23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:1025" customHeight="1" ht="23.7">
       <c r="A24" s="1" t="s">
         <v>77</v>
       </c>
@@ -1387,11 +2654,11 @@
       <c r="G24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:1025" customHeight="1" ht="22.45">
       <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
@@ -1413,11 +2680,11 @@
       <c r="G25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:1025" customHeight="1" ht="23.7">
       <c r="A26" s="1" t="s">
         <v>82</v>
       </c>
@@ -1439,18 +2706,18 @@
       <c r="G26" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A27" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" t="s">
         <v>86</v>
       </c>
       <c r="D27" s="8" t="s">
@@ -1465,11 +2732,11 @@
       <c r="G27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:1025" customHeight="1" ht="22.45">
       <c r="A28" s="1" t="s">
         <v>87</v>
       </c>
@@ -1491,11 +2758,11 @@
       <c r="G28" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="113.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:1025" customHeight="1" ht="113.4">
       <c r="A29" s="1" t="s">
         <v>90</v>
       </c>
@@ -1517,11 +2784,11 @@
       <c r="G29" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="68.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:1025" customHeight="1" ht="68.65">
       <c r="A30" s="1" t="s">
         <v>93</v>
       </c>
@@ -1543,11 +2810,11 @@
       <c r="G30" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="169.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:1025" customHeight="1" ht="169.95">
       <c r="A31" s="1" t="s">
         <v>96</v>
       </c>
@@ -1569,11 +2836,11 @@
       <c r="G31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="H31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:1025" customHeight="1" ht="46.25">
       <c r="A32" s="1" t="s">
         <v>99</v>
       </c>
@@ -1595,11 +2862,11 @@
       <c r="G32" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="H32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:1025" customHeight="1" ht="23.7">
       <c r="A33" s="1" t="s">
         <v>104</v>
       </c>
@@ -1621,11 +2888,11 @@
       <c r="G33" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H33" s="0" t="n">
+      <c r="H33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:1025" customHeight="1" ht="23.7">
       <c r="A34" s="1" t="s">
         <v>107</v>
       </c>
@@ -1647,18 +2914,18 @@
       <c r="G34" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="H34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A35" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" t="s">
         <v>112</v>
       </c>
       <c r="D35" s="8" t="s">
@@ -1673,11 +2940,11 @@
       <c r="G35" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="H35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:1025" customHeight="1" ht="23.7">
       <c r="A36" s="1" t="s">
         <v>113</v>
       </c>
@@ -1699,18 +2966,18 @@
       <c r="G36" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H36" s="0" t="n">
+      <c r="H36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A37" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" t="s">
         <v>117</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" t="s">
         <v>118</v>
       </c>
       <c r="D37" s="8" t="s">
@@ -1725,18 +2992,18 @@
       <c r="G37" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H37" s="0" t="n">
+      <c r="H37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A38" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" t="s">
         <v>121</v>
       </c>
       <c r="D38" s="8" t="s">
@@ -1751,15 +3018,15 @@
       <c r="G38" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H38" s="0" t="n">
+      <c r="H38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:1025" customHeight="1" ht="23.85">
       <c r="A39" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" t="s">
         <v>125</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1777,15 +3044,15 @@
       <c r="G39" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H39" s="0" t="n">
+      <c r="H39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:1025" customHeight="1" ht="23.85">
       <c r="A40" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" t="s">
         <v>128</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -1803,11 +3070,11 @@
       <c r="G40" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H40" s="0" t="n">
+      <c r="H40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A41" s="1" t="s">
         <v>130</v>
       </c>
@@ -1829,11 +3096,11 @@
       <c r="G41" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H41" s="0" t="n">
+      <c r="H41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:1025" customHeight="1" ht="23.85">
       <c r="A42" s="1" t="s">
         <v>134</v>
       </c>
@@ -1855,11 +3122,11 @@
       <c r="G42" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H42" s="0" t="n">
+      <c r="H42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:1025" customHeight="1" ht="23.85">
       <c r="A43" s="1" t="s">
         <v>137</v>
       </c>
@@ -1881,11 +3148,11 @@
       <c r="G43" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H43" s="1" t="n">
+      <c r="H43" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:1025" customHeight="1" ht="23.85">
       <c r="A44" s="1" t="s">
         <v>140</v>
       </c>
@@ -1907,11 +3174,11 @@
       <c r="G44" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H44" s="1" t="n">
+      <c r="H44" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:1025" customHeight="1" ht="23.85">
       <c r="A45" s="1" t="s">
         <v>144</v>
       </c>
@@ -1933,11 +3200,11 @@
       <c r="G45" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H45" s="1" t="n">
+      <c r="H45" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:1025" customHeight="1" ht="23.85">
       <c r="A46" s="1" t="s">
         <v>147</v>
       </c>
@@ -1959,11 +3226,11 @@
       <c r="G46" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H46" s="1" t="n">
+      <c r="H46" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:1025" customHeight="1" ht="23.85">
       <c r="A47" s="1" t="s">
         <v>150</v>
       </c>
@@ -1985,11 +3252,11 @@
       <c r="G47" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="1" t="n">
+      <c r="H47" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:1025" customHeight="1" ht="12.8">
       <c r="A48" s="1" t="s">
         <v>153</v>
       </c>
@@ -2011,11 +3278,11 @@
       <c r="G48" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="H48" s="1" t="n">
+      <c r="H48" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:1025" customHeight="1" ht="35.05">
       <c r="A49" s="1" t="s">
         <v>157</v>
       </c>
@@ -2037,11 +3304,11 @@
       <c r="G49" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="H49" s="1" t="n">
+      <c r="H49" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:1025" customHeight="1" ht="35.05">
       <c r="A50" s="1" t="s">
         <v>160</v>
       </c>
@@ -2063,11 +3330,11 @@
       <c r="G50" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="H50" s="1" t="n">
+      <c r="H50" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:1025" customHeight="1" ht="23.85">
       <c r="A51" s="1" t="s">
         <v>163</v>
       </c>
@@ -2089,11 +3356,11 @@
       <c r="G51" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="H51" s="4" t="n">
+      <c r="H51" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:1025" customHeight="1" ht="35.05">
       <c r="A52" s="1" t="s">
         <v>166</v>
       </c>
@@ -2115,11 +3382,11 @@
       <c r="G52" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="H52" s="4" t="n">
+      <c r="H52" s="4">
         <v>51</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:1025" customHeight="1" ht="23.85">
       <c r="A53" s="1" t="s">
         <v>169</v>
       </c>
@@ -2141,11 +3408,11 @@
       <c r="G53" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H53" s="4" t="n">
+      <c r="H53" s="4">
         <v>52</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:1025" customHeight="1" ht="46.25">
       <c r="A54" s="1" t="s">
         <v>173</v>
       </c>
@@ -2167,11 +3434,11 @@
       <c r="G54" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H54" s="4" t="n">
+      <c r="H54" s="4">
         <v>53</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:1025" customHeight="1" ht="23.85">
       <c r="A55" s="1" t="s">
         <v>176</v>
       </c>
@@ -2193,11 +3460,11 @@
       <c r="G55" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H55" s="4" t="n">
+      <c r="H55" s="4">
         <v>54</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:1025" customHeight="1" ht="35.05">
       <c r="A56" s="1" t="s">
         <v>179</v>
       </c>
@@ -2219,11 +3486,11 @@
       <c r="G56" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H56" s="4" t="n">
+      <c r="H56" s="4">
         <v>55</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:1025" customHeight="1" ht="35.05">
       <c r="A57" s="1" t="s">
         <v>182</v>
       </c>
@@ -2245,32 +3512,71 @@
       <c r="G57" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
+      <c r="H57" s="4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1025" customHeight="1" ht="23.85">
+      <c r="A58" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H58" s="4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1025" customHeight="1" ht="12.8"/>
   </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <dataValidations count="4">
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2:D57" type="list">
+    <dataValidation type="list" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="0" showErrorMessage="0" sqref="D2:D58">
       <formula1>"Mínimo,Importante,Opcional"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E2:E57" type="list">
+    <dataValidation type="list" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="0" showErrorMessage="0" sqref="E2:E58">
       <formula1>"Técnico,Funcional,Información"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F2:F57" type="list">
+    <dataValidation type="list" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="0" showErrorMessage="0" sqref="F2:F58">
       <formula1>"Fácil,Media,Difícil"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G2:G57" type="list">
+    <dataValidation type="list" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="0" showErrorMessage="0" sqref="G2:G58">
       <formula1>"v1,v2,v3"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <hyperlinks>
+    <hyperlink ref="H57" r:id="rId_hyperlink_1"/>
+    <hyperlink ref="H58" r:id="rId_hyperlink_2"/>
+  </hyperlinks>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Añadimos mas documentacion y quitamos archivos que no se usan
</commit_message>
<xml_diff>
--- a/guia/requisitos.xlsx
+++ b/guia/requisitos.xlsx
@@ -2082,7 +2082,7 @@
       <c r="G2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>1</v>
       </c>
     </row>
@@ -2108,7 +2108,7 @@
       <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <v>2</v>
       </c>
     </row>
@@ -2134,7 +2134,7 @@
       <c r="G4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>3</v>
       </c>
     </row>
@@ -2160,7 +2160,7 @@
       <c r="G5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <v>4</v>
       </c>
     </row>
@@ -2186,7 +2186,7 @@
       <c r="G6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <v>5</v>
       </c>
     </row>
@@ -2212,7 +2212,7 @@
       <c r="G7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4">
         <v>6</v>
       </c>
     </row>
@@ -2238,7 +2238,7 @@
       <c r="G8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <v>7</v>
       </c>
     </row>
@@ -2264,7 +2264,7 @@
       <c r="G9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="4">
         <v>8</v>
       </c>
     </row>
@@ -2290,7 +2290,7 @@
       <c r="G10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4">
         <v>9</v>
       </c>
     </row>
@@ -2316,7 +2316,7 @@
       <c r="G11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="4">
         <v>10</v>
       </c>
     </row>
@@ -2342,7 +2342,7 @@
       <c r="G12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="4">
         <v>11</v>
       </c>
     </row>
@@ -2368,7 +2368,7 @@
       <c r="G13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="4">
         <v>12</v>
       </c>
     </row>
@@ -2394,7 +2394,7 @@
       <c r="G14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="4">
         <v>13</v>
       </c>
     </row>
@@ -2420,7 +2420,7 @@
       <c r="G15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2446,7 +2446,7 @@
       <c r="G16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="4">
         <v>15</v>
       </c>
     </row>
@@ -2472,7 +2472,7 @@
       <c r="G17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="4">
         <v>16</v>
       </c>
     </row>
@@ -2498,7 +2498,7 @@
       <c r="G18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="4">
         <v>17</v>
       </c>
     </row>
@@ -2524,7 +2524,7 @@
       <c r="G19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="4">
         <v>18</v>
       </c>
     </row>
@@ -2550,7 +2550,7 @@
       <c r="G20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="4">
         <v>19</v>
       </c>
     </row>
@@ -2576,7 +2576,7 @@
       <c r="G21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="4">
         <v>20</v>
       </c>
     </row>
@@ -2602,7 +2602,7 @@
       <c r="G22" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="4">
         <v>21</v>
       </c>
     </row>
@@ -2628,7 +2628,7 @@
       <c r="G23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="4">
         <v>22</v>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       <c r="G24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="4">
         <v>23</v>
       </c>
     </row>
@@ -2680,7 +2680,7 @@
       <c r="G25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="4">
         <v>24</v>
       </c>
     </row>
@@ -2706,7 +2706,7 @@
       <c r="G26" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="4">
         <v>25</v>
       </c>
     </row>
@@ -2717,7 +2717,7 @@
       <c r="B27" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D27" s="8" t="s">
@@ -2732,7 +2732,7 @@
       <c r="G27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="4">
         <v>26</v>
       </c>
     </row>
@@ -2758,7 +2758,7 @@
       <c r="G28" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="4">
         <v>27</v>
       </c>
     </row>
@@ -2784,7 +2784,7 @@
       <c r="G29" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="4">
         <v>28</v>
       </c>
     </row>
@@ -2810,7 +2810,7 @@
       <c r="G30" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="4">
         <v>29</v>
       </c>
     </row>
@@ -2836,7 +2836,7 @@
       <c r="G31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="4">
         <v>30</v>
       </c>
     </row>
@@ -2862,7 +2862,7 @@
       <c r="G32" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="4">
         <v>31</v>
       </c>
     </row>
@@ -2888,7 +2888,7 @@
       <c r="G33" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="4">
         <v>32</v>
       </c>
     </row>
@@ -2914,7 +2914,7 @@
       <c r="G34" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="4">
         <v>33</v>
       </c>
     </row>
@@ -2925,7 +2925,7 @@
       <c r="B35" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="3" t="s">
         <v>112</v>
       </c>
       <c r="D35" s="8" t="s">
@@ -2940,7 +2940,7 @@
       <c r="G35" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="4">
         <v>34</v>
       </c>
     </row>
@@ -2966,7 +2966,7 @@
       <c r="G36" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="4">
         <v>35</v>
       </c>
     </row>
@@ -2974,10 +2974,10 @@
       <c r="A37" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="3" t="s">
         <v>118</v>
       </c>
       <c r="D37" s="8" t="s">
@@ -2992,7 +2992,7 @@
       <c r="G37" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="4">
         <v>36</v>
       </c>
     </row>
@@ -3000,10 +3000,10 @@
       <c r="A38" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D38" s="8" t="s">
@@ -3018,7 +3018,7 @@
       <c r="G38" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="4">
         <v>37</v>
       </c>
     </row>
@@ -3026,7 +3026,7 @@
       <c r="A39" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -3044,7 +3044,7 @@
       <c r="G39" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="4">
         <v>38</v>
       </c>
     </row>
@@ -3052,7 +3052,7 @@
       <c r="A40" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>128</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -3070,7 +3070,7 @@
       <c r="G40" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="4">
         <v>39</v>
       </c>
     </row>
@@ -3096,7 +3096,7 @@
       <c r="G41" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="4">
         <v>40</v>
       </c>
     </row>
@@ -3122,7 +3122,7 @@
       <c r="G42" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="4">
         <v>41</v>
       </c>
     </row>

</xml_diff>